<commit_message>
Lab4 almost finished but one problem
Problem with the name, kind of same as Thomas but a problem with == iso2
</commit_message>
<xml_diff>
--- a/Data-sheet-STUDENTS-filled.xlsx
+++ b/Data-sheet-STUDENTS-filled.xlsx
@@ -1078,6 +1078,18 @@
       <c r="B2" t="s">
         <v>44</v>
       </c>
+      <c r="D2">
+        <v>51.5</v>
+      </c>
+      <c r="E2">
+        <v>152</v>
+      </c>
+      <c r="F2">
+        <v>2.954762</v>
+      </c>
+      <c r="G2">
+        <v>121</v>
+      </c>
       <c r="H2">
         <v>35.203141190445</v>
       </c>
@@ -1098,6 +1110,33 @@
       </c>
       <c r="Q2" t="s">
         <v>112</v>
+      </c>
+      <c r="R2">
+        <v>16</v>
+      </c>
+      <c r="S2">
+        <v>172</v>
+      </c>
+      <c r="T2">
+        <v>19199437988.8023</v>
+      </c>
+      <c r="U2">
+        <v>590.2695153826051</v>
+      </c>
+      <c r="V2">
+        <v>1.51991126448578</v>
+      </c>
+      <c r="W2">
+        <v>-1.28616720583651</v>
+      </c>
+      <c r="X2">
+        <v>22.6039268726035</v>
+      </c>
+      <c r="Y2">
+        <v>22.4166817955447</v>
+      </c>
+      <c r="Z2">
+        <v>54.9793913318518</v>
       </c>
       <c r="AA2">
         <v>0</v>
@@ -1128,6 +1167,18 @@
       <c r="B3" t="s">
         <v>45</v>
       </c>
+      <c r="D3">
+        <v>66.5</v>
+      </c>
+      <c r="E3">
+        <v>52</v>
+      </c>
+      <c r="F3">
+        <v>6.828571000000001</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
       <c r="H3">
         <v>2.21645910864918</v>
       </c>
@@ -1148,6 +1199,33 @@
       </c>
       <c r="Q3">
         <v>156.1011</v>
+      </c>
+      <c r="R3">
+        <v>36</v>
+      </c>
+      <c r="S3">
+        <v>99</v>
+      </c>
+      <c r="T3">
+        <v>11455595709.1413</v>
+      </c>
+      <c r="U3">
+        <v>3965.01680558488</v>
+      </c>
+      <c r="V3">
+        <v>2.55999999999999</v>
+      </c>
+      <c r="W3">
+        <v>2.71928006930717</v>
+      </c>
+      <c r="X3">
+        <v>22.0492060503358</v>
+      </c>
+      <c r="Y3">
+        <v>26.1513054666415</v>
+      </c>
+      <c r="Z3">
+        <v>51.7994884830226</v>
       </c>
       <c r="AA3">
         <v>0</v>
@@ -1178,6 +1256,18 @@
       <c r="B4" t="s">
         <v>46</v>
       </c>
+      <c r="D4">
+        <v>67.7</v>
+      </c>
+      <c r="E4">
+        <v>47</v>
+      </c>
+      <c r="F4">
+        <v>5.57619</v>
+      </c>
+      <c r="G4">
+        <v>61</v>
+      </c>
       <c r="H4">
         <v>6.27539489392694</v>
       </c>
@@ -1198,6 +1288,33 @@
       </c>
       <c r="Q4" t="s">
         <v>112</v>
+      </c>
+      <c r="R4">
+        <v>35</v>
+      </c>
+      <c r="S4">
+        <v>105</v>
+      </c>
+      <c r="T4">
+        <v>10561401185.098</v>
+      </c>
+      <c r="U4">
+        <v>3499.80421759862</v>
+      </c>
+      <c r="V4">
+        <v>3.00000000125773</v>
+      </c>
+      <c r="W4">
+        <v>2.60550443640113</v>
+      </c>
+      <c r="X4">
+        <v>19.3520404502788</v>
+      </c>
+      <c r="Y4">
+        <v>28.7222907426849</v>
+      </c>
+      <c r="Z4">
+        <v>51.9256688070363</v>
       </c>
       <c r="AA4">
         <v>0</v>
@@ -1228,6 +1345,18 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
+      <c r="D5">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
+        <v>4.127381</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
       <c r="H5">
         <v>7.57184668387459</v>
       </c>
@@ -1248,6 +1377,33 @@
       </c>
       <c r="Q5" t="s">
         <v>112</v>
+      </c>
+      <c r="R5">
+        <v>25</v>
+      </c>
+      <c r="S5">
+        <v>152</v>
+      </c>
+      <c r="T5">
+        <v>53047140347.4527</v>
+      </c>
+      <c r="U5">
+        <v>5496.34464026248</v>
+      </c>
+      <c r="V5">
+        <v>1.09999999999999</v>
+      </c>
+      <c r="W5">
+        <v>-0.117953780347179</v>
+      </c>
+      <c r="X5">
+        <v>6.79136800335426</v>
+      </c>
+      <c r="Y5">
+        <v>36.9931249761771</v>
+      </c>
+      <c r="Z5">
+        <v>56.2155070204686</v>
       </c>
       <c r="AA5">
         <v>0</v>
@@ -1278,6 +1434,18 @@
       <c r="B6" t="s">
         <v>48</v>
       </c>
+      <c r="D6">
+        <v>66.40000000000001</v>
+      </c>
+      <c r="E6">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <v>4.616667</v>
+      </c>
+      <c r="G6">
+        <v>89</v>
+      </c>
       <c r="H6">
         <v>27.3860911270983</v>
       </c>
@@ -1298,6 +1466,33 @@
       </c>
       <c r="Q6">
         <v>368.90235</v>
+      </c>
+      <c r="R6">
+        <v>36</v>
+      </c>
+      <c r="S6">
+        <v>99</v>
+      </c>
+      <c r="T6">
+        <v>32221489361.7021</v>
+      </c>
+      <c r="U6">
+        <v>23395.7476902684</v>
+      </c>
+      <c r="V6">
+        <v>2.92656721719055</v>
+      </c>
+      <c r="W6">
+        <v>1.78261235365325</v>
+      </c>
+      <c r="X6">
+        <v>25.4640636454042</v>
+      </c>
+      <c r="Y6">
+        <v>41.3708969169512</v>
+      </c>
+      <c r="Z6">
+        <v>58.3286560442681</v>
       </c>
       <c r="AA6">
         <v>0</v>
@@ -1328,6 +1523,18 @@
       <c r="B7" t="s">
         <v>49</v>
       </c>
+      <c r="D7">
+        <v>55.6</v>
+      </c>
+      <c r="E7">
+        <v>121</v>
+      </c>
+      <c r="F7">
+        <v>5.111905</v>
+      </c>
+      <c r="G7">
+        <v>79</v>
+      </c>
       <c r="H7">
         <v>28.9230080455078</v>
       </c>
@@ -1348,6 +1555,33 @@
       </c>
       <c r="Q7" t="s">
         <v>112</v>
+      </c>
+      <c r="R7">
+        <v>26</v>
+      </c>
+      <c r="S7">
+        <v>149</v>
+      </c>
+      <c r="T7">
+        <v>195078665827.565</v>
+      </c>
+      <c r="U7">
+        <v>1211.70153057661</v>
+      </c>
+      <c r="V7">
+        <v>6.55263331602802</v>
+      </c>
+      <c r="W7">
+        <v>5.2831474252867</v>
+      </c>
+      <c r="X7">
+        <v>14.8497291534782</v>
+      </c>
+      <c r="Y7">
+        <v>28.1463235005595</v>
+      </c>
+      <c r="Z7">
+        <v>56.3462045652581</v>
       </c>
       <c r="AA7">
         <v>0</v>
@@ -1378,6 +1612,18 @@
       <c r="B8" t="s">
         <v>50</v>
       </c>
+      <c r="D8">
+        <v>57.9</v>
+      </c>
+      <c r="E8">
+        <v>104</v>
+      </c>
+      <c r="F8">
+        <v>4.720238</v>
+      </c>
+      <c r="G8">
+        <v>86</v>
+      </c>
       <c r="H8">
         <v>8.200619287304651</v>
       </c>
@@ -1398,6 +1644,33 @@
       </c>
       <c r="Q8" t="s">
         <v>112</v>
+      </c>
+      <c r="R8">
+        <v>44</v>
+      </c>
+      <c r="S8">
+        <v>70</v>
+      </c>
+      <c r="T8">
+        <v>54608962634.9908</v>
+      </c>
+      <c r="U8">
+        <v>5740.45649479562</v>
+      </c>
+      <c r="V8">
+        <v>-3.88769850231654</v>
+      </c>
+      <c r="W8">
+        <v>-4.19079626799829</v>
+      </c>
+      <c r="X8">
+        <v>0.300447038780779</v>
+      </c>
+      <c r="Y8">
+        <v>40.1472592179596</v>
+      </c>
+      <c r="Z8">
+        <v>52.0569624048448</v>
       </c>
       <c r="AA8">
         <v>0</v>
@@ -1428,6 +1701,18 @@
       <c r="B9" t="s">
         <v>51</v>
       </c>
+      <c r="D9">
+        <v>62.9</v>
+      </c>
+      <c r="E9">
+        <v>74</v>
+      </c>
+      <c r="F9">
+        <v>6.247619</v>
+      </c>
+      <c r="G9">
+        <v>45</v>
+      </c>
       <c r="H9">
         <v>2.84050136682242</v>
       </c>
@@ -1448,6 +1733,33 @@
       </c>
       <c r="Q9" t="s">
         <v>112</v>
+      </c>
+      <c r="R9">
+        <v>68</v>
+      </c>
+      <c r="S9">
+        <v>25</v>
+      </c>
+      <c r="T9">
+        <v>1962221695.69413</v>
+      </c>
+      <c r="U9">
+        <v>2532.45446832741</v>
+      </c>
+      <c r="V9">
+        <v>3.25425473889356</v>
+      </c>
+      <c r="W9">
+        <v>1.9453698350496</v>
+      </c>
+      <c r="X9">
+        <v>2.77654622035025</v>
+      </c>
+      <c r="Y9">
+        <v>42.0790242339736</v>
+      </c>
+      <c r="Z9">
+        <v>40.8652126344372</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -1478,6 +1790,18 @@
       <c r="B10" t="s">
         <v>52</v>
       </c>
+      <c r="D10">
+        <v>61.9</v>
+      </c>
+      <c r="E10">
+        <v>83</v>
+      </c>
+      <c r="F10">
+        <v>6.282143</v>
+      </c>
+      <c r="G10">
+        <v>43</v>
+      </c>
       <c r="H10">
         <v>0.000155359665070619</v>
       </c>
@@ -1498,6 +1822,33 @@
       </c>
       <c r="Q10">
         <v>463.89852</v>
+      </c>
+      <c r="R10">
+        <v>38</v>
+      </c>
+      <c r="S10">
+        <v>89</v>
+      </c>
+      <c r="T10">
+        <v>15995392117.9473</v>
+      </c>
+      <c r="U10">
+        <v>4197.80730449044</v>
+      </c>
+      <c r="V10">
+        <v>3.15757629916973</v>
+      </c>
+      <c r="W10">
+        <v>3.35081997115292</v>
+      </c>
+      <c r="X10">
+        <v>5.13820734776027</v>
+      </c>
+      <c r="Y10">
+        <v>27.13001108395</v>
+      </c>
+      <c r="Z10">
+        <v>65.7655687803434</v>
       </c>
       <c r="AA10">
         <v>0</v>
@@ -1528,6 +1879,12 @@
       <c r="B11" t="s">
         <v>53</v>
       </c>
+      <c r="D11">
+        <v>65.09999999999999</v>
+      </c>
+      <c r="E11">
+        <v>63</v>
+      </c>
       <c r="H11" t="s">
         <v>112</v>
       </c>
@@ -1548,6 +1905,24 @@
       </c>
       <c r="Q11">
         <v>283.4311</v>
+      </c>
+      <c r="R11">
+        <v>63</v>
+      </c>
+      <c r="S11">
+        <v>31</v>
+      </c>
+      <c r="T11">
+        <v>15492035784.4207</v>
+      </c>
+      <c r="U11">
+        <v>36607.9278817468</v>
+      </c>
+      <c r="V11">
+        <v>6.49999990951666</v>
+      </c>
+      <c r="W11">
+        <v>-1.86228579260282</v>
       </c>
       <c r="AA11">
         <v>0</v>
@@ -1578,6 +1953,18 @@
       <c r="B12" t="s">
         <v>54</v>
       </c>
+      <c r="D12">
+        <v>69</v>
+      </c>
+      <c r="E12">
+        <v>37</v>
+      </c>
+      <c r="F12">
+        <v>7.8</v>
+      </c>
+      <c r="G12">
+        <v>17</v>
+      </c>
       <c r="H12">
         <v>0.06885960996340169</v>
       </c>
@@ -1598,6 +1985,33 @@
       </c>
       <c r="Q12">
         <v>2130.54538</v>
+      </c>
+      <c r="R12">
+        <v>42</v>
+      </c>
+      <c r="S12">
+        <v>77</v>
+      </c>
+      <c r="T12">
+        <v>48952959079.5738</v>
+      </c>
+      <c r="U12">
+        <v>6819.86910816324</v>
+      </c>
+      <c r="V12">
+        <v>2.96713547854921</v>
+      </c>
+      <c r="W12">
+        <v>3.62623786163006</v>
+      </c>
+      <c r="X12">
+        <v>7.79577837719564</v>
+      </c>
+      <c r="Y12">
+        <v>27.6133062083995</v>
+      </c>
+      <c r="Z12">
+        <v>67.24848644384021</v>
       </c>
       <c r="AA12">
         <v>0</v>
@@ -1632,13 +2046,13 @@
         <v>43328</v>
       </c>
       <c r="D13">
-        <v>58.7</v>
+        <v>57.8</v>
       </c>
       <c r="E13">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F13">
-        <v>4</v>
+        <v>3.997619</v>
       </c>
       <c r="G13">
         <v>103</v>
@@ -1671,7 +2085,7 @@
         <v>30.37447</v>
       </c>
       <c r="R13">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S13">
         <v>161</v>
@@ -1683,19 +2097,19 @@
         <v>1158.68990352486</v>
       </c>
       <c r="V13">
-        <v>0.07036087179364769</v>
+        <v>7.03608717936477</v>
       </c>
       <c r="W13">
-        <v>0.053199601045789</v>
+        <v>5.3199601045789</v>
       </c>
       <c r="X13">
-        <v>0.159416995164261</v>
+        <v>15.9416995164261</v>
       </c>
       <c r="Y13">
-        <v>0.294173723333596</v>
+        <v>29.4173723333596</v>
       </c>
       <c r="Z13">
-        <v>0.423334790133704</v>
+        <v>42.3334790133704</v>
       </c>
       <c r="AA13">
         <v>0.876925508631561</v>
@@ -1753,6 +2167,18 @@
       <c r="B14" t="s">
         <v>56</v>
       </c>
+      <c r="D14">
+        <v>58.4</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>5.016666000000001</v>
+      </c>
+      <c r="G14">
+        <v>81</v>
+      </c>
       <c r="H14">
         <v>3.89434134127694</v>
       </c>
@@ -1773,6 +2199,12 @@
       </c>
       <c r="Q14">
         <v>1234.7788</v>
+      </c>
+      <c r="R14">
+        <v>39</v>
+      </c>
+      <c r="S14">
+        <v>87</v>
       </c>
       <c r="AC14">
         <v>24</v>
@@ -1809,6 +2241,18 @@
       <c r="B15" t="s">
         <v>57</v>
       </c>
+      <c r="D15">
+        <v>61.4</v>
+      </c>
+      <c r="E15">
+        <v>86</v>
+      </c>
+      <c r="F15">
+        <v>8.067857999999999</v>
+      </c>
+      <c r="G15">
+        <v>14</v>
+      </c>
       <c r="H15">
         <v>-0.0376305545169416</v>
       </c>
@@ -1829,6 +2273,30 @@
       </c>
       <c r="Q15">
         <v>1865.44318</v>
+      </c>
+      <c r="R15">
+        <v>48</v>
+      </c>
+      <c r="S15">
+        <v>60</v>
+      </c>
+      <c r="T15">
+        <v>48732003674.38</v>
+      </c>
+      <c r="U15">
+        <v>11535.8293558997</v>
+      </c>
+      <c r="V15">
+        <v>1.64461325883687</v>
+      </c>
+      <c r="W15">
+        <v>1.98111041119844</v>
+      </c>
+      <c r="Y15">
+        <v>26.2052927095021</v>
+      </c>
+      <c r="Z15">
+        <v>69.50386606472389</v>
       </c>
       <c r="AA15">
         <v>0</v>
@@ -1859,6 +2327,18 @@
       <c r="B16" t="s">
         <v>58</v>
       </c>
+      <c r="D16">
+        <v>73.7</v>
+      </c>
+      <c r="E16">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <v>9.521428999999999</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
       <c r="H16">
         <v>0.819566734190984</v>
       </c>
@@ -1879,6 +2359,33 @@
       </c>
       <c r="Q16">
         <v>3689.9158</v>
+      </c>
+      <c r="R16">
+        <v>59</v>
+      </c>
+      <c r="S16">
+        <v>38</v>
+      </c>
+      <c r="T16">
+        <v>181811026983.078</v>
+      </c>
+      <c r="U16">
+        <v>17231.2817109642</v>
+      </c>
+      <c r="V16">
+        <v>4.19804965676525</v>
+      </c>
+      <c r="W16">
+        <v>3.94255198007787</v>
+      </c>
+      <c r="X16">
+        <v>28.2491486532701</v>
+      </c>
+      <c r="Y16">
+        <v>38.091385170647</v>
+      </c>
+      <c r="Z16">
+        <v>59.5250579376435</v>
       </c>
       <c r="AA16">
         <v>0</v>
@@ -1909,6 +2416,12 @@
       <c r="B17" t="s">
         <v>59</v>
       </c>
+      <c r="D17">
+        <v>44.2</v>
+      </c>
+      <c r="E17">
+        <v>172</v>
+      </c>
       <c r="H17">
         <v>4.77991862435917</v>
       </c>
@@ -1929,6 +2442,27 @@
       </c>
       <c r="Q17" t="s">
         <v>112</v>
+      </c>
+      <c r="R17">
+        <v>35</v>
+      </c>
+      <c r="S17">
+        <v>105</v>
+      </c>
+      <c r="T17">
+        <v>1412377919.12175</v>
+      </c>
+      <c r="U17">
+        <v>1134.42642789183</v>
+      </c>
+      <c r="V17">
+        <v>4.251</v>
+      </c>
+      <c r="W17">
+        <v>1.49545736958994</v>
+      </c>
+      <c r="X17">
+        <v>17.0557631315892</v>
       </c>
       <c r="AA17">
         <v>0</v>
@@ -1959,6 +2493,18 @@
       <c r="B18" t="s">
         <v>60</v>
       </c>
+      <c r="D18">
+        <v>52.5</v>
+      </c>
+      <c r="E18">
+        <v>144</v>
+      </c>
+      <c r="F18">
+        <v>4.278572</v>
+      </c>
+      <c r="G18">
+        <v>96</v>
+      </c>
       <c r="H18">
         <v>6.8490016570956</v>
       </c>
@@ -1979,6 +2525,33 @@
       </c>
       <c r="Q18">
         <v>669.39201</v>
+      </c>
+      <c r="R18">
+        <v>35</v>
+      </c>
+      <c r="S18">
+        <v>105</v>
+      </c>
+      <c r="T18">
+        <v>330778550716.746</v>
+      </c>
+      <c r="U18">
+        <v>3614.74676616271</v>
+      </c>
+      <c r="V18">
+        <v>4.2</v>
+      </c>
+      <c r="W18">
+        <v>2.00412035727904</v>
+      </c>
+      <c r="X18">
+        <v>11.1816471975681</v>
+      </c>
+      <c r="Y18">
+        <v>36.3195006150812</v>
+      </c>
+      <c r="Z18">
+        <v>52.498864387308</v>
       </c>
       <c r="AA18">
         <v>0</v>
@@ -2009,6 +2582,18 @@
       <c r="B19" t="s">
         <v>61</v>
       </c>
+      <c r="D19">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="E19">
+        <v>15</v>
+      </c>
+      <c r="F19">
+        <v>9.517857000000001</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
       <c r="H19">
         <v>0.039428987382724</v>
       </c>
@@ -2029,6 +2614,30 @@
       </c>
       <c r="Q19">
         <v>3568.9415</v>
+      </c>
+      <c r="R19">
+        <v>73</v>
+      </c>
+      <c r="S19">
+        <v>18</v>
+      </c>
+      <c r="T19">
+        <v>22691482754.7965</v>
+      </c>
+      <c r="U19">
+        <v>17295.36383043</v>
+      </c>
+      <c r="V19">
+        <v>1.06784053106526</v>
+      </c>
+      <c r="W19">
+        <v>1.26404493826149</v>
+      </c>
+      <c r="Y19">
+        <v>26.7491961759834</v>
+      </c>
+      <c r="Z19">
+        <v>69.7459447339573</v>
       </c>
       <c r="AA19">
         <v>0</v>
@@ -2060,7 +2669,10 @@
         <v>62</v>
       </c>
       <c r="D20">
-        <v>37</v>
+        <v>63.8</v>
+      </c>
+      <c r="E20">
+        <v>71</v>
       </c>
       <c r="H20">
         <v>-0.0232445343314451</v>
@@ -2082,6 +2694,12 @@
       </c>
       <c r="Q20">
         <v>4441.07429</v>
+      </c>
+      <c r="R20">
+        <v>72</v>
+      </c>
+      <c r="S20">
+        <v>21</v>
       </c>
       <c r="AA20">
         <v>0</v>
@@ -2118,6 +2736,18 @@
       <c r="B21" t="s">
         <v>63</v>
       </c>
+      <c r="D21">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="E21">
+        <v>16</v>
+      </c>
+      <c r="F21">
+        <v>6.417857</v>
+      </c>
+      <c r="G21">
+        <v>42</v>
+      </c>
       <c r="H21">
         <v>0.757021008880042</v>
       </c>
@@ -2138,6 +2768,33 @@
       </c>
       <c r="Q21">
         <v>1339.70815</v>
+      </c>
+      <c r="R21">
+        <v>58</v>
+      </c>
+      <c r="S21">
+        <v>41</v>
+      </c>
+      <c r="T21">
+        <v>13965385801.7891</v>
+      </c>
+      <c r="U21">
+        <v>3795.97330845042</v>
+      </c>
+      <c r="V21">
+        <v>2.77492809454047</v>
+      </c>
+      <c r="W21">
+        <v>4.11583501178372</v>
+      </c>
+      <c r="X21">
+        <v>10.2665463273775</v>
+      </c>
+      <c r="Y21">
+        <v>24.5206288020114</v>
+      </c>
+      <c r="Z21">
+        <v>66.2902111459188</v>
       </c>
       <c r="AA21">
         <v>0</v>
@@ -2169,7 +2826,10 @@
         <v>64</v>
       </c>
       <c r="D22">
-        <v>34</v>
+        <v>73.5</v>
+      </c>
+      <c r="E22">
+        <v>24</v>
       </c>
       <c r="H22">
         <v>0.0212485657218138</v>
@@ -2191,6 +2851,12 @@
       </c>
       <c r="Q22">
         <v>5036.17985</v>
+      </c>
+      <c r="R22">
+        <v>80</v>
+      </c>
+      <c r="S22">
+        <v>11</v>
       </c>
       <c r="AA22">
         <v>0</v>
@@ -2233,6 +2899,18 @@
       <c r="B23" t="s">
         <v>65</v>
       </c>
+      <c r="D23">
+        <v>65</v>
+      </c>
+      <c r="E23">
+        <v>64</v>
+      </c>
+      <c r="F23">
+        <v>7.432142999999999</v>
+      </c>
+      <c r="G23">
+        <v>18</v>
+      </c>
       <c r="H23">
         <v>-0.000144686648107121</v>
       </c>
@@ -2253,6 +2931,24 @@
       </c>
       <c r="Q23">
         <v>2924.01661</v>
+      </c>
+      <c r="R23">
+        <v>46</v>
+      </c>
+      <c r="S23">
+        <v>64</v>
+      </c>
+      <c r="T23">
+        <v>120687138088.121</v>
+      </c>
+      <c r="U23">
+        <v>12259.1150279573</v>
+      </c>
+      <c r="V23">
+        <v>2.93891579055648</v>
+      </c>
+      <c r="W23">
+        <v>3.16667475247256</v>
       </c>
       <c r="AA23">
         <v>0</v>
@@ -2283,6 +2979,12 @@
       <c r="B24" t="s">
         <v>66</v>
       </c>
+      <c r="D24">
+        <v>55.2</v>
+      </c>
+      <c r="E24">
+        <v>129</v>
+      </c>
       <c r="H24" t="s">
         <v>112</v>
       </c>
@@ -2303,6 +3005,18 @@
       </c>
       <c r="Q24" t="s">
         <v>112</v>
+      </c>
+      <c r="T24">
+        <v>2073542978208.77</v>
+      </c>
+      <c r="U24">
+        <v>1581.58891324619</v>
+      </c>
+      <c r="V24">
+        <v>7.57013036787396</v>
+      </c>
+      <c r="W24">
+        <v>6.27712454663818</v>
       </c>
       <c r="AA24">
         <v>0</v>
@@ -2333,6 +3047,18 @@
       <c r="B25" t="s">
         <v>67</v>
       </c>
+      <c r="D25">
+        <v>65.8</v>
+      </c>
+      <c r="E25">
+        <v>56</v>
+      </c>
+      <c r="F25">
+        <v>6.25</v>
+      </c>
+      <c r="G25">
+        <v>45</v>
+      </c>
       <c r="H25">
         <v>2.56897518332382</v>
       </c>
@@ -2353,6 +3079,33 @@
       </c>
       <c r="Q25">
         <v>215.72807</v>
+      </c>
+      <c r="R25">
+        <v>38</v>
+      </c>
+      <c r="S25">
+        <v>89</v>
+      </c>
+      <c r="T25">
+        <v>861933968740.332</v>
+      </c>
+      <c r="U25">
+        <v>3346.48703949478</v>
+      </c>
+      <c r="V25">
+        <v>4.7939213038221</v>
+      </c>
+      <c r="W25">
+        <v>3.52896031266474</v>
+      </c>
+      <c r="X25">
+        <v>13.520732350571</v>
+      </c>
+      <c r="Y25">
+        <v>40.0148073054757</v>
+      </c>
+      <c r="Z25">
+        <v>43.3238451323323</v>
       </c>
       <c r="AA25">
         <v>0</v>
@@ -2383,6 +3136,18 @@
       <c r="B26" t="s">
         <v>68</v>
       </c>
+      <c r="D26">
+        <v>51.1</v>
+      </c>
+      <c r="E26">
+        <v>155</v>
+      </c>
+      <c r="F26">
+        <v>3.154762</v>
+      </c>
+      <c r="G26">
+        <v>118</v>
+      </c>
       <c r="H26">
         <v>20.6964502542622</v>
       </c>
@@ -2403,6 +3168,12 @@
       </c>
       <c r="Q26">
         <v>671.02399</v>
+      </c>
+      <c r="R26">
+        <v>28</v>
+      </c>
+      <c r="S26">
+        <v>138</v>
       </c>
       <c r="AA26">
         <v>0</v>
@@ -2433,6 +3204,12 @@
       <c r="B27" t="s">
         <v>69</v>
       </c>
+      <c r="F27">
+        <v>3.746428</v>
+      </c>
+      <c r="G27">
+        <v>107</v>
+      </c>
       <c r="H27">
         <v>14.105211130071</v>
       </c>
@@ -2453,6 +3230,24 @@
       </c>
       <c r="Q27">
         <v>103.92502</v>
+      </c>
+      <c r="R27">
+        <v>18</v>
+      </c>
+      <c r="S27">
+        <v>168</v>
+      </c>
+      <c r="T27">
+        <v>168606686710.642</v>
+      </c>
+      <c r="U27">
+        <v>4629.07663359338</v>
+      </c>
+      <c r="V27">
+        <v>2.09999999999999</v>
+      </c>
+      <c r="W27">
+        <v>-1.12390085273492</v>
       </c>
       <c r="AA27">
         <v>0</v>
@@ -2483,6 +3278,12 @@
       <c r="B28" t="s">
         <v>70</v>
       </c>
+      <c r="D28">
+        <v>72.8</v>
+      </c>
+      <c r="E28">
+        <v>27</v>
+      </c>
       <c r="H28">
         <v>0.962752553897723</v>
       </c>
@@ -2503,6 +3304,24 @@
       </c>
       <c r="Q28">
         <v>8250.474179999999</v>
+      </c>
+      <c r="R28">
+        <v>61</v>
+      </c>
+      <c r="S28">
+        <v>34</v>
+      </c>
+      <c r="T28">
+        <v>296075434804.981</v>
+      </c>
+      <c r="U28">
+        <v>35329.5110979167</v>
+      </c>
+      <c r="V28">
+        <v>2.48807622448481</v>
+      </c>
+      <c r="W28">
+        <v>0.473878077120403</v>
       </c>
       <c r="AA28">
         <v>0</v>
@@ -2533,6 +3352,18 @@
       <c r="B29" t="s">
         <v>71</v>
       </c>
+      <c r="D29">
+        <v>66.5</v>
+      </c>
+      <c r="E29">
+        <v>53</v>
+      </c>
+      <c r="F29">
+        <v>5.219048</v>
+      </c>
+      <c r="G29">
+        <v>72</v>
+      </c>
       <c r="H29">
         <v>7.00619344737872</v>
       </c>
@@ -2553,6 +3384,33 @@
       </c>
       <c r="Q29">
         <v>601.0913</v>
+      </c>
+      <c r="R29">
+        <v>49</v>
+      </c>
+      <c r="S29">
+        <v>58</v>
+      </c>
+      <c r="T29">
+        <v>37517410299.2739</v>
+      </c>
+      <c r="U29">
+        <v>4940.04583805643</v>
+      </c>
+      <c r="V29">
+        <v>2.38268662851466</v>
+      </c>
+      <c r="W29">
+        <v>-0.0232006201219406</v>
+      </c>
+      <c r="X29">
+        <v>4.17398422334225</v>
+      </c>
+      <c r="Y29">
+        <v>29.6406318271146</v>
+      </c>
+      <c r="Z29">
+        <v>66.18538394954329</v>
       </c>
       <c r="AA29">
         <v>0</v>
@@ -2583,6 +3441,18 @@
       <c r="B30" t="s">
         <v>72</v>
       </c>
+      <c r="D30">
+        <v>65.40000000000001</v>
+      </c>
+      <c r="E30">
+        <v>59</v>
+      </c>
+      <c r="F30">
+        <v>4.703571</v>
+      </c>
+      <c r="G30">
+        <v>88</v>
+      </c>
       <c r="H30">
         <v>5.29951905118019</v>
       </c>
@@ -2603,6 +3473,33 @@
       </c>
       <c r="Q30">
         <v>661.5947</v>
+      </c>
+      <c r="R30">
+        <v>31</v>
+      </c>
+      <c r="S30">
+        <v>124</v>
+      </c>
+      <c r="T30">
+        <v>184360630555.504</v>
+      </c>
+      <c r="U30">
+        <v>10508.3964031895</v>
+      </c>
+      <c r="V30">
+        <v>1.20000000000036</v>
+      </c>
+      <c r="W30">
+        <v>-0.270354373879556</v>
+      </c>
+      <c r="X30">
+        <v>9.189160052069809</v>
+      </c>
+      <c r="Y30">
+        <v>33.2279211309936</v>
+      </c>
+      <c r="Z30">
+        <v>61.7647613416438</v>
       </c>
       <c r="AA30">
         <v>0</v>
@@ -2633,6 +3530,18 @@
       <c r="B31" t="s">
         <v>73</v>
       </c>
+      <c r="D31">
+        <v>60.8</v>
+      </c>
+      <c r="E31">
+        <v>90</v>
+      </c>
+      <c r="F31">
+        <v>5.607143</v>
+      </c>
+      <c r="G31">
+        <v>60</v>
+      </c>
       <c r="H31">
         <v>66.8067226890756</v>
       </c>
@@ -2653,6 +3562,27 @@
       </c>
       <c r="Q31">
         <v>491.81342</v>
+      </c>
+      <c r="R31">
+        <v>41</v>
+      </c>
+      <c r="S31">
+        <v>78</v>
+      </c>
+      <c r="T31">
+        <v>112811565304.088</v>
+      </c>
+      <c r="U31">
+        <v>28984.6433890283</v>
+      </c>
+      <c r="V31">
+        <v>-0.40000000000002</v>
+      </c>
+      <c r="W31">
+        <v>-3.95688421333904</v>
+      </c>
+      <c r="X31">
+        <v>0.136286425345325</v>
       </c>
       <c r="AA31">
         <v>0</v>
@@ -2683,6 +3613,18 @@
       <c r="B32" t="s">
         <v>74</v>
       </c>
+      <c r="D32">
+        <v>62.3</v>
+      </c>
+      <c r="E32">
+        <v>79</v>
+      </c>
+      <c r="F32">
+        <v>5.896429</v>
+      </c>
+      <c r="G32">
+        <v>55</v>
+      </c>
       <c r="H32">
         <v>17.6152097175161</v>
       </c>
@@ -2703,6 +3645,33 @@
       </c>
       <c r="Q32" t="s">
         <v>112</v>
+      </c>
+      <c r="R32">
+        <v>29</v>
+      </c>
+      <c r="S32">
+        <v>132</v>
+      </c>
+      <c r="T32">
+        <v>6571853849.00585</v>
+      </c>
+      <c r="U32">
+        <v>1103.2153515202</v>
+      </c>
+      <c r="V32">
+        <v>3.46928079781574</v>
+      </c>
+      <c r="W32">
+        <v>1.35890349096086</v>
+      </c>
+      <c r="X32">
+        <v>10.2</v>
+      </c>
+      <c r="Y32">
+        <v>26.9157155736444</v>
+      </c>
+      <c r="Z32">
+        <v>57.1425849099294</v>
       </c>
       <c r="AA32">
         <v>0</v>
@@ -2733,6 +3702,18 @@
       <c r="B33" t="s">
         <v>75</v>
       </c>
+      <c r="D33">
+        <v>57.4</v>
+      </c>
+      <c r="E33">
+        <v>110</v>
+      </c>
+      <c r="F33">
+        <v>3.851191</v>
+      </c>
+      <c r="G33">
+        <v>106</v>
+      </c>
       <c r="H33" t="s">
         <v>112</v>
       </c>
@@ -2753,6 +3734,30 @@
       </c>
       <c r="Q33">
         <v>15.82603</v>
+      </c>
+      <c r="R33">
+        <v>29</v>
+      </c>
+      <c r="S33">
+        <v>132</v>
+      </c>
+      <c r="T33">
+        <v>12327488340.7341</v>
+      </c>
+      <c r="U33">
+        <v>1812.32676524824</v>
+      </c>
+      <c r="V33">
+        <v>6.99522551975515</v>
+      </c>
+      <c r="W33">
+        <v>5.22210261113469</v>
+      </c>
+      <c r="Y33">
+        <v>30.8744568625836</v>
+      </c>
+      <c r="Z33">
+        <v>41.8820332815012</v>
       </c>
       <c r="AA33">
         <v>0</v>
@@ -2783,6 +3788,18 @@
       <c r="B34" t="s">
         <v>76</v>
       </c>
+      <c r="D34">
+        <v>70.40000000000001</v>
+      </c>
+      <c r="E34">
+        <v>35</v>
+      </c>
+      <c r="F34">
+        <v>8.678572000000001</v>
+      </c>
+      <c r="G34">
+        <v>8</v>
+      </c>
       <c r="H34">
         <v>0.07553723668970749</v>
       </c>
@@ -2803,6 +3820,27 @@
       </c>
       <c r="Q34">
         <v>1785.94326</v>
+      </c>
+      <c r="R34">
+        <v>58</v>
+      </c>
+      <c r="S34">
+        <v>41</v>
+      </c>
+      <c r="T34">
+        <v>27035266718.4208</v>
+      </c>
+      <c r="U34">
+        <v>13664.9414278021</v>
+      </c>
+      <c r="V34">
+        <v>1.88691229576618</v>
+      </c>
+      <c r="W34">
+        <v>2.67700398843398</v>
+      </c>
+      <c r="X34">
+        <v>4.29084122577397</v>
       </c>
       <c r="AA34">
         <v>0</v>
@@ -2833,6 +3871,18 @@
       <c r="B35" t="s">
         <v>77</v>
       </c>
+      <c r="D35">
+        <v>51.1</v>
+      </c>
+      <c r="E35">
+        <v>154</v>
+      </c>
+      <c r="F35">
+        <v>5.147619000000001</v>
+      </c>
+      <c r="G35">
+        <v>74</v>
+      </c>
       <c r="H35">
         <v>6.04488095511726</v>
       </c>
@@ -2853,6 +3903,33 @@
       </c>
       <c r="Q35" t="s">
         <v>112</v>
+      </c>
+      <c r="R35">
+        <v>28</v>
+      </c>
+      <c r="S35">
+        <v>138</v>
+      </c>
+      <c r="T35">
+        <v>47102873631.8408</v>
+      </c>
+      <c r="U35">
+        <v>8050.75075624426</v>
+      </c>
+      <c r="V35">
+        <v>1.50856704175307</v>
+      </c>
+      <c r="W35">
+        <v>-2.63188400844915</v>
+      </c>
+      <c r="X35">
+        <v>27.2435098559153</v>
+      </c>
+      <c r="Y35">
+        <v>20.6709620663426</v>
+      </c>
+      <c r="Z35">
+        <v>73.764035595287</v>
       </c>
       <c r="AA35">
         <v>0</v>
@@ -2883,6 +3960,18 @@
       <c r="B36" t="s">
         <v>78</v>
       </c>
+      <c r="D36">
+        <v>74.2</v>
+      </c>
+      <c r="E36">
+        <v>21</v>
+      </c>
+      <c r="F36">
+        <v>9.242857000000001</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
       <c r="H36">
         <v>0.711031058816326</v>
       </c>
@@ -2903,6 +3992,27 @@
       </c>
       <c r="Q36">
         <v>3013.18515</v>
+      </c>
+      <c r="R36">
+        <v>59</v>
+      </c>
+      <c r="S36">
+        <v>38</v>
+      </c>
+      <c r="T36">
+        <v>41243983586.5587</v>
+      </c>
+      <c r="U36">
+        <v>14172.2210702975</v>
+      </c>
+      <c r="V36">
+        <v>1.59377460567481</v>
+      </c>
+      <c r="W36">
+        <v>2.36764979271824</v>
+      </c>
+      <c r="X36">
+        <v>5.56500233837039</v>
       </c>
       <c r="AA36">
         <v>0</v>
@@ -2933,6 +4043,18 @@
       <c r="B37" t="s">
         <v>79</v>
       </c>
+      <c r="D37">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="E37">
+        <v>33</v>
+      </c>
+      <c r="F37">
+        <v>6.760714999999999</v>
+      </c>
+      <c r="G37">
+        <v>31</v>
+      </c>
       <c r="H37">
         <v>4.65911362142491</v>
       </c>
@@ -2953,6 +4075,33 @@
       </c>
       <c r="Q37">
         <v>728.95025</v>
+      </c>
+      <c r="R37">
+        <v>37</v>
+      </c>
+      <c r="S37">
+        <v>93</v>
+      </c>
+      <c r="T37">
+        <v>10086021260.9944</v>
+      </c>
+      <c r="U37">
+        <v>4852.65784744443</v>
+      </c>
+      <c r="V37">
+        <v>3.66528037380903</v>
+      </c>
+      <c r="W37">
+        <v>3.5242305579618</v>
+      </c>
+      <c r="X37">
+        <v>8.43079391258197</v>
+      </c>
+      <c r="Y37">
+        <v>26.1379004321792</v>
+      </c>
+      <c r="Z37">
+        <v>62.7006451456147</v>
       </c>
       <c r="AA37">
         <v>0</v>
@@ -2987,13 +4136,13 @@
         <v>43328</v>
       </c>
       <c r="D38">
-        <v>74.5</v>
+        <v>74</v>
       </c>
       <c r="E38">
         <v>22</v>
       </c>
       <c r="F38">
-        <v>6</v>
+        <v>5.99881</v>
       </c>
       <c r="G38">
         <v>53</v>
@@ -3032,7 +4181,7 @@
         <v>47</v>
       </c>
       <c r="S38">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T38">
         <v>296217641787.223</v>
@@ -3041,19 +4190,16 @@
         <v>9766.16575200497</v>
       </c>
       <c r="V38">
-        <v>0.0495237060557724</v>
+        <v>4.95237060557724</v>
       </c>
       <c r="W38">
-        <v>0.0346789577381521</v>
-      </c>
-      <c r="X38">
-        <v>0.0352706191844887</v>
+        <v>3.46789577381521</v>
       </c>
       <c r="Y38">
-        <v>0.39123658674467</v>
+        <v>39.123658674467</v>
       </c>
       <c r="Z38">
-        <v>0.443003497343713</v>
+        <v>44.3003497343713</v>
       </c>
       <c r="AA38">
         <v>0.8695107032728717</v>
@@ -3114,6 +4260,12 @@
       <c r="B39" t="s">
         <v>81</v>
       </c>
+      <c r="D39">
+        <v>53.2</v>
+      </c>
+      <c r="E39">
+        <v>141</v>
+      </c>
       <c r="H39">
         <v>17.845797817127</v>
       </c>
@@ -3134,6 +4286,27 @@
       </c>
       <c r="Q39" t="s">
         <v>112</v>
+      </c>
+      <c r="R39">
+        <v>31</v>
+      </c>
+      <c r="S39">
+        <v>124</v>
+      </c>
+      <c r="T39">
+        <v>3142812004.19099</v>
+      </c>
+      <c r="U39">
+        <v>7681.07576733719</v>
+      </c>
+      <c r="V39">
+        <v>1.51388419597605</v>
+      </c>
+      <c r="W39">
+        <v>-0.511366955012065</v>
+      </c>
+      <c r="X39">
+        <v>4.75907978438019</v>
       </c>
       <c r="AA39">
         <v>0</v>
@@ -3164,6 +4337,18 @@
       <c r="B40" t="s">
         <v>82</v>
       </c>
+      <c r="D40">
+        <v>59.1</v>
+      </c>
+      <c r="E40">
+        <v>97</v>
+      </c>
+      <c r="F40">
+        <v>5.957143</v>
+      </c>
+      <c r="G40">
+        <v>54</v>
+      </c>
       <c r="H40">
         <v>3.42323285739468</v>
       </c>
@@ -3184,6 +4369,30 @@
       </c>
       <c r="Q40">
         <v>723.88211</v>
+      </c>
+      <c r="R40">
+        <v>33</v>
+      </c>
+      <c r="S40">
+        <v>117</v>
+      </c>
+      <c r="T40">
+        <v>6551161404.09357</v>
+      </c>
+      <c r="U40">
+        <v>1843.24280182141</v>
+      </c>
+      <c r="V40">
+        <v>-0.5</v>
+      </c>
+      <c r="W40">
+        <v>-0.437094241942518</v>
+      </c>
+      <c r="Y40">
+        <v>17.9488668324983</v>
+      </c>
+      <c r="Z40">
+        <v>68.22066088456251</v>
       </c>
       <c r="AA40">
         <v>0</v>
@@ -3214,6 +4423,18 @@
       <c r="B41" t="s">
         <v>83</v>
       </c>
+      <c r="D41">
+        <v>55.4</v>
+      </c>
+      <c r="E41">
+        <v>126</v>
+      </c>
+      <c r="F41">
+        <v>6.592857</v>
+      </c>
+      <c r="G41">
+        <v>34</v>
+      </c>
       <c r="H41">
         <v>13.5021655958073</v>
       </c>
@@ -3234,6 +4455,33 @@
       </c>
       <c r="Q41" t="s">
         <v>112</v>
+      </c>
+      <c r="R41">
+        <v>37</v>
+      </c>
+      <c r="S41">
+        <v>93</v>
+      </c>
+      <c r="T41">
+        <v>11757940908.6277</v>
+      </c>
+      <c r="U41">
+        <v>3973.43983362286</v>
+      </c>
+      <c r="V41">
+        <v>2.29544361018836</v>
+      </c>
+      <c r="W41">
+        <v>0.592451978660804</v>
+      </c>
+      <c r="X41">
+        <v>11.1614544222061</v>
+      </c>
+      <c r="Y41">
+        <v>34.0705088562784</v>
+      </c>
+      <c r="Z41">
+        <v>51.0797619902436</v>
       </c>
       <c r="AA41">
         <v>0</v>
@@ -3264,6 +4512,18 @@
       <c r="B42" t="s">
         <v>84</v>
       </c>
+      <c r="D42">
+        <v>60.5</v>
+      </c>
+      <c r="E42">
+        <v>92</v>
+      </c>
+      <c r="F42">
+        <v>7.346429</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
+      </c>
       <c r="H42" t="s">
         <v>112</v>
       </c>
@@ -3284,6 +4544,33 @@
       </c>
       <c r="Q42">
         <v>714.26867</v>
+      </c>
+      <c r="R42">
+        <v>45</v>
+      </c>
+      <c r="S42">
+        <v>67</v>
+      </c>
+      <c r="T42">
+        <v>3992640233.17019</v>
+      </c>
+      <c r="U42">
+        <v>6415.03408351413</v>
+      </c>
+      <c r="V42">
+        <v>3.37469381321137</v>
+      </c>
+      <c r="W42">
+        <v>3.27869168427566</v>
+      </c>
+      <c r="X42">
+        <v>5.00731752736254</v>
+      </c>
+      <c r="Y42">
+        <v>20.3</v>
+      </c>
+      <c r="Z42">
+        <v>69.5</v>
       </c>
       <c r="AA42">
         <v>0</v>
@@ -3314,6 +4601,18 @@
       <c r="B43" t="s">
         <v>85</v>
       </c>
+      <c r="D43">
+        <v>53.6</v>
+      </c>
+      <c r="E43">
+        <v>139</v>
+      </c>
+      <c r="F43">
+        <v>3.375</v>
+      </c>
+      <c r="G43">
+        <v>111</v>
+      </c>
       <c r="H43">
         <v>9.003221505158089</v>
       </c>
@@ -3334,6 +4633,27 @@
       </c>
       <c r="Q43">
         <v>29.07968</v>
+      </c>
+      <c r="R43">
+        <v>29</v>
+      </c>
+      <c r="S43">
+        <v>132</v>
+      </c>
+      <c r="T43">
+        <v>64865515159.2277</v>
+      </c>
+      <c r="U43">
+        <v>1203.50538655951</v>
+      </c>
+      <c r="V43">
+        <v>6.99127097835952</v>
+      </c>
+      <c r="W43">
+        <v>6.07813464292907</v>
+      </c>
+      <c r="X43">
+        <v>15.5074719341824</v>
       </c>
       <c r="AA43">
         <v>0</v>
@@ -3364,6 +4684,18 @@
       <c r="B44" t="s">
         <v>86</v>
       </c>
+      <c r="D44">
+        <v>53.8</v>
+      </c>
+      <c r="E44">
+        <v>136</v>
+      </c>
+      <c r="F44">
+        <v>4.521429</v>
+      </c>
+      <c r="G44">
+        <v>92</v>
+      </c>
       <c r="H44">
         <v>17.7700383177162</v>
       </c>
@@ -3384,6 +4716,33 @@
       </c>
       <c r="Q44">
         <v>61.05915</v>
+      </c>
+      <c r="R44">
+        <v>31</v>
+      </c>
+      <c r="S44">
+        <v>124</v>
+      </c>
+      <c r="T44">
+        <v>20880545907.4264</v>
+      </c>
+      <c r="U44">
+        <v>732.298716316243</v>
+      </c>
+      <c r="V44">
+        <v>3.36295318337802</v>
+      </c>
+      <c r="W44">
+        <v>2.13415578359164</v>
+      </c>
+      <c r="X44">
+        <v>13.830656461372</v>
+      </c>
+      <c r="Y44">
+        <v>15.6633876230348</v>
+      </c>
+      <c r="Z44">
+        <v>51.5505780300137</v>
       </c>
       <c r="AA44">
         <v>0</v>
@@ -3414,6 +4773,18 @@
       <c r="B45" t="s">
         <v>87</v>
       </c>
+      <c r="D45">
+        <v>61</v>
+      </c>
+      <c r="E45">
+        <v>88</v>
+      </c>
+      <c r="F45">
+        <v>4.428572</v>
+      </c>
+      <c r="G45">
+        <v>93</v>
+      </c>
       <c r="H45" t="s">
         <v>112</v>
       </c>
@@ -3434,6 +4805,24 @@
       </c>
       <c r="Q45">
         <v>243.96162</v>
+      </c>
+      <c r="R45">
+        <v>52</v>
+      </c>
+      <c r="S45">
+        <v>53</v>
+      </c>
+      <c r="T45">
+        <v>70254876462.9389</v>
+      </c>
+      <c r="U45">
+        <v>15645.0807292348</v>
+      </c>
+      <c r="V45">
+        <v>3.49999999999999</v>
+      </c>
+      <c r="W45">
+        <v>-2.36546119944124</v>
       </c>
       <c r="AA45">
         <v>0</v>
@@ -3464,6 +4853,18 @@
       <c r="B46" t="s">
         <v>88</v>
       </c>
+      <c r="D46">
+        <v>55</v>
+      </c>
+      <c r="E46">
+        <v>131</v>
+      </c>
+      <c r="F46">
+        <v>4.010715</v>
+      </c>
+      <c r="G46">
+        <v>102</v>
+      </c>
       <c r="H46" t="s">
         <v>112</v>
       </c>
@@ -3484,6 +4885,33 @@
       </c>
       <c r="Q46">
         <v>354.1302</v>
+      </c>
+      <c r="R46">
+        <v>33</v>
+      </c>
+      <c r="S46">
+        <v>117</v>
+      </c>
+      <c r="T46">
+        <v>269971498118.442</v>
+      </c>
+      <c r="U46">
+        <v>1428.98863660717</v>
+      </c>
+      <c r="V46">
+        <v>5.53810056237647</v>
+      </c>
+      <c r="W46">
+        <v>3.37030826529043</v>
+      </c>
+      <c r="X46">
+        <v>3.50485909005935</v>
+      </c>
+      <c r="Y46">
+        <v>18.9918473602083</v>
+      </c>
+      <c r="Z46">
+        <v>55.5440889943875</v>
       </c>
       <c r="AA46">
         <v>0</v>
@@ -3514,6 +4942,18 @@
       <c r="B47" t="s">
         <v>89</v>
       </c>
+      <c r="D47">
+        <v>63.8</v>
+      </c>
+      <c r="E47">
+        <v>70</v>
+      </c>
+      <c r="F47">
+        <v>6.471429</v>
+      </c>
+      <c r="G47">
+        <v>38</v>
+      </c>
       <c r="H47">
         <v>20.3576079552952</v>
       </c>
@@ -3534,6 +4974,33 @@
       </c>
       <c r="Q47">
         <v>187.65898</v>
+      </c>
+      <c r="R47">
+        <v>36</v>
+      </c>
+      <c r="S47">
+        <v>99</v>
+      </c>
+      <c r="T47">
+        <v>291965336390.95</v>
+      </c>
+      <c r="U47">
+        <v>2899.37527818265</v>
+      </c>
+      <c r="V47">
+        <v>5.80572866285858</v>
+      </c>
+      <c r="W47">
+        <v>4.16588236832258</v>
+      </c>
+      <c r="X47">
+        <v>4.63007864310703</v>
+      </c>
+      <c r="Y47">
+        <v>30.8898334926965</v>
+      </c>
+      <c r="Z47">
+        <v>58.843620179926</v>
       </c>
       <c r="AA47">
         <v>0</v>
@@ -3564,6 +5031,18 @@
       <c r="B48" t="s">
         <v>90</v>
       </c>
+      <c r="D48">
+        <v>67.8</v>
+      </c>
+      <c r="E48">
+        <v>46</v>
+      </c>
+      <c r="F48">
+        <v>8.578571</v>
+      </c>
+      <c r="G48">
+        <v>10</v>
+      </c>
       <c r="H48">
         <v>0.128545876239141</v>
       </c>
@@ -3584,6 +5063,33 @@
       </c>
       <c r="Q48">
         <v>2528.03773</v>
+      </c>
+      <c r="R48">
+        <v>60</v>
+      </c>
+      <c r="S48">
+        <v>36</v>
+      </c>
+      <c r="T48">
+        <v>474783393022.947</v>
+      </c>
+      <c r="U48">
+        <v>12494.4661900747</v>
+      </c>
+      <c r="V48">
+        <v>3.64971913068008</v>
+      </c>
+      <c r="W48">
+        <v>3.68310842296589</v>
+      </c>
+      <c r="X48">
+        <v>7.10442013570666</v>
+      </c>
+      <c r="Y48">
+        <v>33.541179641684</v>
+      </c>
+      <c r="Z48">
+        <v>63.6822741379658</v>
       </c>
       <c r="AA48">
         <v>0</v>
@@ -3614,6 +5120,18 @@
       <c r="B49" t="s">
         <v>91</v>
       </c>
+      <c r="D49">
+        <v>72.59999999999999</v>
+      </c>
+      <c r="E49">
+        <v>28</v>
+      </c>
+      <c r="F49">
+        <v>5.884524</v>
+      </c>
+      <c r="G49">
+        <v>56</v>
+      </c>
       <c r="H49" t="s">
         <v>112</v>
       </c>
@@ -3634,6 +5152,33 @@
       </c>
       <c r="Q49">
         <v>603.79063</v>
+      </c>
+      <c r="R49">
+        <v>62</v>
+      </c>
+      <c r="S49">
+        <v>33</v>
+      </c>
+      <c r="T49">
+        <v>166907692307.692</v>
+      </c>
+      <c r="U49">
+        <v>74667.1970705737</v>
+      </c>
+      <c r="V49">
+        <v>3.58277342974473</v>
+      </c>
+      <c r="W49">
+        <v>0.6500161136278</v>
+      </c>
+      <c r="X49">
+        <v>2.38355689170941</v>
+      </c>
+      <c r="Y49">
+        <v>55.7613934134812</v>
+      </c>
+      <c r="Z49">
+        <v>44.1023201611735</v>
       </c>
       <c r="AA49">
         <v>0</v>
@@ -3664,6 +5209,12 @@
       <c r="B50" t="s">
         <v>92</v>
       </c>
+      <c r="D50">
+        <v>68.59999999999999</v>
+      </c>
+      <c r="E50">
+        <v>42</v>
+      </c>
       <c r="H50">
         <v>0.035332354395594</v>
       </c>
@@ -3684,6 +5235,30 @@
       </c>
       <c r="Q50">
         <v>890.17367</v>
+      </c>
+      <c r="R50">
+        <v>47</v>
+      </c>
+      <c r="S50">
+        <v>61</v>
+      </c>
+      <c r="T50">
+        <v>177954489851.961</v>
+      </c>
+      <c r="U50">
+        <v>8972.92251840971</v>
+      </c>
+      <c r="V50">
+        <v>3.73668357850366</v>
+      </c>
+      <c r="W50">
+        <v>4.13730059924066</v>
+      </c>
+      <c r="Y50">
+        <v>26.4496323093554</v>
+      </c>
+      <c r="Z50">
+        <v>68.7912879062644</v>
       </c>
       <c r="AA50">
         <v>0</v>
@@ -3714,6 +5289,18 @@
       <c r="B51" t="s">
         <v>93</v>
       </c>
+      <c r="D51">
+        <v>58.9</v>
+      </c>
+      <c r="E51">
+        <v>98</v>
+      </c>
+      <c r="F51">
+        <v>5.310715</v>
+      </c>
+      <c r="G51">
+        <v>70</v>
+      </c>
       <c r="H51">
         <v>6.21762623104324</v>
       </c>
@@ -3734,6 +5321,30 @@
       </c>
       <c r="Q51">
         <v>2851.70985</v>
+      </c>
+      <c r="R51">
+        <v>28</v>
+      </c>
+      <c r="S51">
+        <v>138</v>
+      </c>
+      <c r="T51">
+        <v>1326015096948.19</v>
+      </c>
+      <c r="U51">
+        <v>9057.11306037766</v>
+      </c>
+      <c r="V51">
+        <v>-3.72667344001421</v>
+      </c>
+      <c r="W51">
+        <v>-3.9340216039501</v>
+      </c>
+      <c r="Y51">
+        <v>32.6045564415853</v>
+      </c>
+      <c r="Z51">
+        <v>62.7653649153076</v>
       </c>
       <c r="AA51">
         <v>0</v>
@@ -3764,6 +5375,18 @@
       <c r="B52" t="s">
         <v>94</v>
       </c>
+      <c r="D52">
+        <v>60.7</v>
+      </c>
+      <c r="E52">
+        <v>91</v>
+      </c>
+      <c r="F52">
+        <v>4.265476</v>
+      </c>
+      <c r="G52">
+        <v>97</v>
+      </c>
       <c r="H52">
         <v>23.0173047901435</v>
       </c>
@@ -3784,6 +5407,33 @@
       </c>
       <c r="Q52" t="s">
         <v>112</v>
+      </c>
+      <c r="R52">
+        <v>49</v>
+      </c>
+      <c r="S52">
+        <v>58</v>
+      </c>
+      <c r="T52">
+        <v>646001866666.667</v>
+      </c>
+      <c r="U52">
+        <v>20481.7453220484</v>
+      </c>
+      <c r="V52">
+        <v>3.48565641322274</v>
+      </c>
+      <c r="W52">
+        <v>1.34041487086908</v>
+      </c>
+      <c r="X52">
+        <v>9.46274605767656</v>
+      </c>
+      <c r="Y52">
+        <v>45.8979065901564</v>
+      </c>
+      <c r="Z52">
+        <v>51.8379926249955</v>
       </c>
       <c r="AA52">
         <v>0</v>
@@ -3814,6 +5464,18 @@
       <c r="B53" t="s">
         <v>95</v>
       </c>
+      <c r="D53">
+        <v>63.9</v>
+      </c>
+      <c r="E53">
+        <v>69</v>
+      </c>
+      <c r="F53">
+        <v>7.403571</v>
+      </c>
+      <c r="G53">
+        <v>19</v>
+      </c>
       <c r="H53">
         <v>5.06221866137756</v>
       </c>
@@ -3834,6 +5496,33 @@
       </c>
       <c r="Q53">
         <v>2079.19966</v>
+      </c>
+      <c r="R53">
+        <v>39</v>
+      </c>
+      <c r="S53">
+        <v>87</v>
+      </c>
+      <c r="T53">
+        <v>36513027127.6723</v>
+      </c>
+      <c r="U53">
+        <v>5143.94992561858</v>
+      </c>
+      <c r="V53">
+        <v>0.726074886537418</v>
+      </c>
+      <c r="W53">
+        <v>1.18483227762383</v>
+      </c>
+      <c r="X53">
+        <v>32.7860343469515</v>
+      </c>
+      <c r="Y53">
+        <v>30.1053105407539</v>
+      </c>
+      <c r="Z53">
+        <v>60.4319434015695</v>
       </c>
       <c r="AA53">
         <v>0</v>
@@ -3864,6 +5553,18 @@
       <c r="B54" t="s">
         <v>96</v>
       </c>
+      <c r="D54">
+        <v>89.40000000000001</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>7.154762</v>
+      </c>
+      <c r="G54">
+        <v>24</v>
+      </c>
       <c r="H54">
         <v>0.07150825205228679</v>
       </c>
@@ -3884,6 +5585,27 @@
       </c>
       <c r="Q54">
         <v>6729.67978</v>
+      </c>
+      <c r="R54">
+        <v>85</v>
+      </c>
+      <c r="S54">
+        <v>3</v>
+      </c>
+      <c r="T54">
+        <v>292739307535.642</v>
+      </c>
+      <c r="U54">
+        <v>52888.7446717529</v>
+      </c>
+      <c r="V54">
+        <v>2.008372345195</v>
+      </c>
+      <c r="W54">
+        <v>0.805319025620818</v>
+      </c>
+      <c r="X54">
+        <v>18.2634544720488</v>
       </c>
       <c r="AA54">
         <v>0</v>
@@ -3914,6 +5636,18 @@
       <c r="B55" t="s">
         <v>97</v>
       </c>
+      <c r="D55">
+        <v>65</v>
+      </c>
+      <c r="E55">
+        <v>65</v>
+      </c>
+      <c r="F55">
+        <v>8.585713999999999</v>
+      </c>
+      <c r="G55">
+        <v>9</v>
+      </c>
       <c r="H55">
         <v>6.64156553388789e-05</v>
       </c>
@@ -3934,6 +5668,33 @@
       </c>
       <c r="Q55">
         <v>2794.96048</v>
+      </c>
+      <c r="R55">
+        <v>50</v>
+      </c>
+      <c r="S55">
+        <v>57</v>
+      </c>
+      <c r="T55">
+        <v>86581789952.3123</v>
+      </c>
+      <c r="U55">
+        <v>15962.5722388828</v>
+      </c>
+      <c r="V55">
+        <v>3.59502093291218</v>
+      </c>
+      <c r="W55">
+        <v>3.49186614856126</v>
+      </c>
+      <c r="X55">
+        <v>8.67951186043066</v>
+      </c>
+      <c r="Y55">
+        <v>34.384839708011</v>
+      </c>
+      <c r="Z55">
+        <v>61.5662156970323</v>
       </c>
       <c r="AA55">
         <v>0</v>
@@ -3964,6 +5725,18 @@
       <c r="B56" t="s">
         <v>98</v>
       </c>
+      <c r="D56">
+        <v>65.5</v>
+      </c>
+      <c r="E56">
+        <v>58</v>
+      </c>
+      <c r="F56">
+        <v>9.178572000000001</v>
+      </c>
+      <c r="G56">
+        <v>6</v>
+      </c>
       <c r="H56">
         <v>0.8082799979161081</v>
       </c>
@@ -3984,6 +5757,33 @@
       </c>
       <c r="Q56">
         <v>4467.84001</v>
+      </c>
+      <c r="R56">
+        <v>60</v>
+      </c>
+      <c r="S56">
+        <v>36</v>
+      </c>
+      <c r="T56">
+        <v>42746980843.0904</v>
+      </c>
+      <c r="U56">
+        <v>20713.0747463331</v>
+      </c>
+      <c r="V56">
+        <v>2.87916089867399</v>
+      </c>
+      <c r="W56">
+        <v>2.79002881614979</v>
+      </c>
+      <c r="X56">
+        <v>4.04894459495668</v>
+      </c>
+      <c r="Y56">
+        <v>33.0631143382462</v>
+      </c>
+      <c r="Z56">
+        <v>64.7589486699775</v>
       </c>
       <c r="AA56">
         <v>0</v>
@@ -4014,6 +5814,18 @@
       <c r="B57" t="s">
         <v>99</v>
       </c>
+      <c r="D57">
+        <v>56.4</v>
+      </c>
+      <c r="E57">
+        <v>115</v>
+      </c>
+      <c r="F57">
+        <v>6.614285000000001</v>
+      </c>
+      <c r="G57">
+        <v>33</v>
+      </c>
       <c r="H57">
         <v>22.0548905792486</v>
       </c>
@@ -4034,6 +5846,33 @@
       </c>
       <c r="Q57">
         <v>106.98058</v>
+      </c>
+      <c r="R57">
+        <v>38</v>
+      </c>
+      <c r="S57">
+        <v>89</v>
+      </c>
+      <c r="T57">
+        <v>82316172384.325</v>
+      </c>
+      <c r="U57">
+        <v>3926.17439589454</v>
+      </c>
+      <c r="V57">
+        <v>4.78598456723587</v>
+      </c>
+      <c r="W57">
+        <v>3.81139394477039</v>
+      </c>
+      <c r="X57">
+        <v>2.26410078484809</v>
+      </c>
+      <c r="Y57">
+        <v>30.7102356990977</v>
+      </c>
+      <c r="Z57">
+        <v>60.6102524404716</v>
       </c>
       <c r="AA57">
         <v>0</v>
@@ -4064,6 +5903,12 @@
       <c r="B58" t="s">
         <v>100</v>
       </c>
+      <c r="F58">
+        <v>1.571429</v>
+      </c>
+      <c r="G58">
+        <v>128</v>
+      </c>
       <c r="H58" t="s">
         <v>112</v>
       </c>
@@ -4084,6 +5929,12 @@
       </c>
       <c r="Q58">
         <v>87.37663000000001</v>
+      </c>
+      <c r="R58">
+        <v>13</v>
+      </c>
+      <c r="S58">
+        <v>178</v>
       </c>
       <c r="AA58">
         <v>0</v>
@@ -4114,6 +5965,18 @@
       <c r="B59" t="s">
         <v>101</v>
       </c>
+      <c r="D59">
+        <v>55.6</v>
+      </c>
+      <c r="E59">
+        <v>122</v>
+      </c>
+      <c r="F59">
+        <v>3.313095</v>
+      </c>
+      <c r="G59">
+        <v>115</v>
+      </c>
       <c r="H59">
         <v>15.9437469869174</v>
       </c>
@@ -4134,6 +5997,27 @@
       </c>
       <c r="Q59" t="s">
         <v>112</v>
+      </c>
+      <c r="R59">
+        <v>25</v>
+      </c>
+      <c r="S59">
+        <v>152</v>
+      </c>
+      <c r="T59">
+        <v>7853450374.0001</v>
+      </c>
+      <c r="U59">
+        <v>925.91188767081</v>
+      </c>
+      <c r="V59">
+        <v>4.19999999999999</v>
+      </c>
+      <c r="W59">
+        <v>1.91479670425866</v>
+      </c>
+      <c r="X59">
+        <v>2.17793699177633</v>
       </c>
       <c r="AA59">
         <v>0</v>
@@ -4165,7 +6049,16 @@
         <v>102</v>
       </c>
       <c r="D60">
-        <v>62</v>
+        <v>68.3</v>
+      </c>
+      <c r="E60">
+        <v>43</v>
+      </c>
+      <c r="F60">
+        <v>4.714286</v>
+      </c>
+      <c r="G60">
+        <v>87</v>
       </c>
       <c r="H60">
         <v>3.952756587923</v>
@@ -4187,6 +6080,12 @@
       </c>
       <c r="Q60">
         <v>1210.35067</v>
+      </c>
+      <c r="R60">
+        <v>36</v>
+      </c>
+      <c r="S60">
+        <v>99</v>
       </c>
       <c r="AA60">
         <v>0</v>
@@ -4217,6 +6116,18 @@
       <c r="B61" t="s">
         <v>103</v>
       </c>
+      <c r="D61">
+        <v>77.59999999999999</v>
+      </c>
+      <c r="E61">
+        <v>9</v>
+      </c>
+      <c r="F61">
+        <v>6.071429</v>
+      </c>
+      <c r="G61">
+        <v>52</v>
+      </c>
       <c r="H61">
         <v>0.381747427685012</v>
       </c>
@@ -4237,6 +6148,24 @@
       </c>
       <c r="Q61">
         <v>2406.57322</v>
+      </c>
+      <c r="R61">
+        <v>70</v>
+      </c>
+      <c r="S61">
+        <v>23</v>
+      </c>
+      <c r="T61">
+        <v>370292716133.424</v>
+      </c>
+      <c r="U61">
+        <v>40438.3763627115</v>
+      </c>
+      <c r="V61">
+        <v>3.18267819490927</v>
+      </c>
+      <c r="W61">
+        <v>2.38461774621288</v>
       </c>
       <c r="AA61">
         <v>0</v>
@@ -4267,6 +6196,18 @@
       <c r="B62" t="s">
         <v>104</v>
       </c>
+      <c r="D62">
+        <v>64.59999999999999</v>
+      </c>
+      <c r="E62">
+        <v>68</v>
+      </c>
+      <c r="F62">
+        <v>6.167857</v>
+      </c>
+      <c r="G62">
+        <v>51</v>
+      </c>
       <c r="H62">
         <v>2.50452275929646</v>
       </c>
@@ -4287,6 +6228,27 @@
       </c>
       <c r="Q62">
         <v>1385.75729</v>
+      </c>
+      <c r="R62">
+        <v>41</v>
+      </c>
+      <c r="S62">
+        <v>78</v>
+      </c>
+      <c r="T62">
+        <v>718221078308.824</v>
+      </c>
+      <c r="U62">
+        <v>9130.02606479616</v>
+      </c>
+      <c r="W62">
+        <v>2.47524471544042</v>
+      </c>
+      <c r="Y62">
+        <v>26.4912091465332</v>
+      </c>
+      <c r="Z62">
+        <v>64.9192896320277</v>
       </c>
       <c r="AA62">
         <v>0</v>
@@ -4317,6 +6279,18 @@
       <c r="B63" t="s">
         <v>105</v>
       </c>
+      <c r="D63">
+        <v>48.4</v>
+      </c>
+      <c r="E63">
+        <v>164</v>
+      </c>
+      <c r="F63">
+        <v>3.139286</v>
+      </c>
+      <c r="G63">
+        <v>119</v>
+      </c>
       <c r="H63" t="s">
         <v>112</v>
       </c>
@@ -4337,6 +6311,27 @@
       </c>
       <c r="Q63" t="s">
         <v>112</v>
+      </c>
+      <c r="R63">
+        <v>20</v>
+      </c>
+      <c r="S63">
+        <v>161</v>
+      </c>
+      <c r="T63">
+        <v>37334232257.1429</v>
+      </c>
+      <c r="U63">
+        <v>6947.84002260404</v>
+      </c>
+      <c r="V63">
+        <v>3.98485920209721</v>
+      </c>
+      <c r="W63">
+        <v>5.1856911041976</v>
+      </c>
+      <c r="X63">
+        <v>8.58950122143913</v>
       </c>
       <c r="AA63">
         <v>0</v>
@@ -4368,7 +6363,10 @@
         <v>106</v>
       </c>
       <c r="D64">
-        <v>55</v>
+        <v>78.90000000000001</v>
+      </c>
+      <c r="E64">
+        <v>7</v>
       </c>
       <c r="H64">
         <v>0.0477474161684688</v>
@@ -4390,6 +6388,12 @@
       </c>
       <c r="Q64">
         <v>4376.95773</v>
+      </c>
+      <c r="R64">
+        <v>80</v>
+      </c>
+      <c r="S64">
+        <v>11</v>
       </c>
       <c r="AA64">
         <v>0</v>
@@ -4420,6 +6424,12 @@
       <c r="B65" t="s">
         <v>107</v>
       </c>
+      <c r="D65">
+        <v>76.8</v>
+      </c>
+      <c r="E65">
+        <v>12</v>
+      </c>
       <c r="H65">
         <v>2.64259418024106</v>
       </c>
@@ -4440,6 +6450,12 @@
       </c>
       <c r="Q65">
         <v>4256.29052</v>
+      </c>
+      <c r="R65">
+        <v>71</v>
+      </c>
+      <c r="S65">
+        <v>22</v>
       </c>
       <c r="AA65">
         <v>0</v>
@@ -4470,6 +6486,18 @@
       <c r="B66" t="s">
         <v>108</v>
       </c>
+      <c r="D66">
+        <v>52.3</v>
+      </c>
+      <c r="E66">
+        <v>147</v>
+      </c>
+      <c r="F66">
+        <v>6.539286</v>
+      </c>
+      <c r="G66">
+        <v>36</v>
+      </c>
       <c r="H66">
         <v>3.99768085531341</v>
       </c>
@@ -4490,6 +6518,30 @@
       </c>
       <c r="Q66">
         <v>994.07744</v>
+      </c>
+      <c r="R66">
+        <v>32</v>
+      </c>
+      <c r="S66">
+        <v>120</v>
+      </c>
+      <c r="T66">
+        <v>90615023323.73531</v>
+      </c>
+      <c r="U66">
+        <v>2114.95471628444</v>
+      </c>
+      <c r="V66">
+        <v>-0.5</v>
+      </c>
+      <c r="W66">
+        <v>-9.57171491891337</v>
+      </c>
+      <c r="Y66">
+        <v>25.9104766821382</v>
+      </c>
+      <c r="Z66">
+        <v>60.0531887054144</v>
       </c>
       <c r="AA66">
         <v>0</v>
@@ -4520,6 +6572,18 @@
       <c r="B67" t="s">
         <v>109</v>
       </c>
+      <c r="D67">
+        <v>53.3</v>
+      </c>
+      <c r="E67">
+        <v>140</v>
+      </c>
+      <c r="F67">
+        <v>3.726191</v>
+      </c>
+      <c r="G67">
+        <v>108</v>
+      </c>
       <c r="H67">
         <v>5.186860136235</v>
       </c>
@@ -4540,6 +6604,33 @@
       </c>
       <c r="Q67">
         <v>496.336</v>
+      </c>
+      <c r="R67">
+        <v>23</v>
+      </c>
+      <c r="S67">
+        <v>158</v>
+      </c>
+      <c r="T67">
+        <v>66732801392.6618</v>
+      </c>
+      <c r="U67">
+        <v>2132.07244181734</v>
+      </c>
+      <c r="V67">
+        <v>7.99999999999994</v>
+      </c>
+      <c r="W67">
+        <v>6.13050048722816</v>
+      </c>
+      <c r="X67">
+        <v>14.0363346124475</v>
+      </c>
+      <c r="Y67">
+        <v>34.6262346289219</v>
+      </c>
+      <c r="Z67">
+        <v>47.1103108990293</v>
       </c>
       <c r="AA67">
         <v>0</v>
@@ -4570,6 +6661,18 @@
       <c r="B68" t="s">
         <v>110</v>
       </c>
+      <c r="D68">
+        <v>55.3</v>
+      </c>
+      <c r="E68">
+        <v>128</v>
+      </c>
+      <c r="F68">
+        <v>4.407143</v>
+      </c>
+      <c r="G68">
+        <v>94</v>
+      </c>
       <c r="H68" t="s">
         <v>112</v>
       </c>
@@ -4590,6 +6693,33 @@
       </c>
       <c r="Q68">
         <v>700.77914</v>
+      </c>
+      <c r="R68">
+        <v>33</v>
+      </c>
+      <c r="S68">
+        <v>117</v>
+      </c>
+      <c r="T68">
+        <v>193599379094.859</v>
+      </c>
+      <c r="U68">
+        <v>2111.13802366815</v>
+      </c>
+      <c r="V68">
+        <v>6.67928878891431</v>
+      </c>
+      <c r="W68">
+        <v>5.54518487347883</v>
+      </c>
+      <c r="X68">
+        <v>16.9922120022076</v>
+      </c>
+      <c r="Y68">
+        <v>33.2500807324448</v>
+      </c>
+      <c r="Z68">
+        <v>39.7332895764278</v>
       </c>
       <c r="AA68">
         <v>0</v>
@@ -4620,6 +6750,12 @@
       <c r="B69" t="s">
         <v>111</v>
       </c>
+      <c r="F69">
+        <v>1.721429</v>
+      </c>
+      <c r="G69">
+        <v>127</v>
+      </c>
       <c r="H69" t="s">
         <v>112</v>
       </c>
@@ -4640,6 +6776,12 @@
       </c>
       <c r="Q69" t="s">
         <v>112</v>
+      </c>
+      <c r="R69">
+        <v>14</v>
+      </c>
+      <c r="S69">
+        <v>176</v>
       </c>
       <c r="AA69">
         <v>0</v>

</xml_diff>